<commit_message>
Purchase BI Report by Imam Hossain With Source\3. Yarn Received Report
</commit_message>
<xml_diff>
--- a/3. Purchase BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Purchase BI by IM from Source).xlsx
+++ b/3. Purchase BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Purchase BI by IM from Source).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\3. Purchase BI Report by Imam Hossain With Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8351638-C33D-4B9E-96E5-13FB10F15C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E4CCB0-3FE8-4481-951C-40533001A617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="2" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="3" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar Date" sheetId="1" r:id="rId1"/>
     <sheet name="Last Refresh Date &amp; Time" sheetId="2" r:id="rId2"/>
     <sheet name="1. Purchase Requisition Status" sheetId="11" r:id="rId3"/>
+    <sheet name="3. Yarn Received Report" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>https://debug.to/899/calendarauto-function-can-not-find-a-base-column-of-datetime-type-in-the-model</t>
   </si>
@@ -2178,6 +2179,996 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Count Name = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(Vw_PO_Receipt[OE or Ring 2]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Polyester Filament Yarn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONCATENATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(Vw_PO_Receipt[OE or Ring 2], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(Vw_PO_Receipt[Count]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Rewinding"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONCATENATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(Vw_PO_Receipt[Count], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" Yarn (Mixed Count)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONCATENATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(Vw_PO_Receipt[Count], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONCATENATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, Vw_PO_Receipt[OE or Ring 2]))</t>
+    </r>
+  </si>
+  <si>
+    <t>                )</t>
+  </si>
+  <si>
+    <t>            )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Count = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PATHITEM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUBSTITUTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Vw_PO_Receipt'[ITEMDESC]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"|"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OE or Ring 2 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONVERT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONTAINSSTRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[ITEMDESC]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"OE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"True"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Open End"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONVERT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONTAINSSTRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[ITEMDESC]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Rewinding"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"True"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Open End"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONVERT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONTAINSSTRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[ITEMDESC]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"D/"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"True"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Polyester Filament Yarn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Ring"</t>
+    </r>
+  </si>
+  <si>
+    <t>)))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total Cost USD = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[UNITCOST]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[QTY]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OE or Ring = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONVERT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CONTAINSSTRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_PO_Receipt[ITEMDESC]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"OE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>STRING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"True"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Open End"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>))</t>
   </si>
 </sst>
 </file>
@@ -2290,7 +3281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2404,12 +3395,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2458,11 +3464,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3079,7 +4091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3F52D-D0C2-44C6-A702-979CF9AC2B30}">
   <dimension ref="A2:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A43" sqref="A43:A44"/>
     </sheetView>
   </sheetViews>
@@ -3126,31 +4138,31 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-    </row>
-    <row r="17" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
     </row>
     <row r="21" spans="1:1" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
@@ -3159,7 +4171,7 @@
     </row>
     <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3226,6 +4238,117 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFF2197-DC2D-40F7-A22A-7E8AE98A7B18}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:1" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="6" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19"/>
+    </row>
+    <row r="23" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>